<commit_message>
chore(packages): - added packages.txt
</commit_message>
<xml_diff>
--- a/check_and_fix_results.xlsx
+++ b/check_and_fix_results.xlsx
@@ -1245,12 +1245,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>fail</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>ran</t>
+          <t>pass</t>
         </is>
       </c>
     </row>

</xml_diff>